<commit_message>
power_dist r4: Checkpoint, most power/gnd routed
</commit_message>
<xml_diff>
--- a/hw/power_dist/LM5066I_Design_Calculator_REV_C.XLSX
+++ b/hw/power_dist/LM5066I_Design_Calculator_REV_C.XLSX
@@ -6017,7 +6017,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7113,11 +7113,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="43852805"/>
-        <c:axId val="60679484"/>
+        <c:axId val="54266612"/>
+        <c:axId val="72212107"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43852805"/>
+        <c:axId val="54266612"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7217,12 +7217,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60679484"/>
+        <c:crossAx val="72212107"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60679484"/>
+        <c:axId val="72212107"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7322,7 +7322,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43852805"/>
+        <c:crossAx val="54266612"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7393,7 +7393,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8801,11 +8801,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="32942623"/>
-        <c:axId val="54143539"/>
+        <c:axId val="14759296"/>
+        <c:axId val="75004980"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32942623"/>
+        <c:axId val="14759296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8899,12 +8899,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54143539"/>
+        <c:crossAx val="75004980"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54143539"/>
+        <c:axId val="75004980"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -8999,7 +8999,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32942623"/>
+        <c:crossAx val="14759296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9062,7 +9062,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9833,11 +9833,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="15511"/>
-        <c:axId val="54900460"/>
+        <c:axId val="28155369"/>
+        <c:axId val="65267046"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="15511"/>
+        <c:axId val="28155369"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -9922,12 +9922,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54900460"/>
+        <c:crossAx val="65267046"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54900460"/>
+        <c:axId val="65267046"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -10022,7 +10022,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15511"/>
+        <c:crossAx val="28155369"/>
         <c:crossesAt val="-1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10085,7 +10085,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -11483,11 +11483,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="88318627"/>
-        <c:axId val="40458723"/>
+        <c:axId val="64298080"/>
+        <c:axId val="14308980"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88318627"/>
+        <c:axId val="64298080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11553,12 +11553,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40458723"/>
+        <c:crossAx val="14308980"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40458723"/>
+        <c:axId val="14308980"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -11635,7 +11635,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88318627"/>
+        <c:crossAx val="64298080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16965,8 +16965,8 @@
   </sheetPr>
   <dimension ref="A1:AU227"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F91" activeCellId="0" sqref="F91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F109" activeCellId="0" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21529,7 +21529,7 @@
         <v>138</v>
       </c>
       <c r="F97" s="157" t="n">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="G97" s="158" t="s">
         <v>40</v>
@@ -21579,7 +21579,7 @@
         <v>139</v>
       </c>
       <c r="F98" s="157" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G98" s="158" t="s">
         <v>40</v>
@@ -21629,7 +21629,7 @@
         <v>141</v>
       </c>
       <c r="F99" s="157" t="n">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G99" s="158" t="s">
         <v>40</v>
@@ -21679,7 +21679,7 @@
         <v>143</v>
       </c>
       <c r="F100" s="157" t="n">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G100" s="158" t="s">
         <v>40</v>
@@ -21727,7 +21727,7 @@
       </c>
       <c r="F101" s="161" t="n">
         <f aca="false">IF(F96="Option A",Equations!F119,Equations!G119)</f>
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="G101" s="158" t="s">
         <v>96</v>
@@ -21775,7 +21775,7 @@
       </c>
       <c r="F102" s="161" t="n">
         <f aca="false">IF(F96="Option A",Equations!F120,Equations!G120)</f>
-        <v>11.4391143911439</v>
+        <v>19.0184049079755</v>
       </c>
       <c r="G102" s="158" t="s">
         <v>96</v>
@@ -21825,7 +21825,7 @@
       </c>
       <c r="F103" s="161" t="n">
         <f aca="false">IF(F96="Option A",Equations!F121,Equations!G121)</f>
-        <v>95.2380952380952</v>
+        <v>142.857142857143</v>
       </c>
       <c r="G103" s="158" t="s">
         <v>96</v>
@@ -21873,7 +21873,7 @@
       </c>
       <c r="F104" s="161" t="n">
         <f aca="false">IF(F96="Option A",Equations!F122,Equations!G122)</f>
-        <v>3.74617387728996</v>
+        <v>6.32748598178919</v>
       </c>
       <c r="G104" s="158" t="s">
         <v>96</v>
@@ -21920,7 +21920,7 @@
         <v>148</v>
       </c>
       <c r="F105" s="157" t="n">
-        <v>150</v>
+        <v>47</v>
       </c>
       <c r="G105" s="158" t="s">
         <v>96</v>
@@ -21967,7 +21967,7 @@
         <v>149</v>
       </c>
       <c r="F106" s="157" t="n">
-        <v>11.5</v>
+        <v>19.1</v>
       </c>
       <c r="G106" s="158" t="s">
         <v>96</v>
@@ -22014,7 +22014,7 @@
         <v>150</v>
       </c>
       <c r="F107" s="157" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="G107" s="158" t="s">
         <v>96</v>
@@ -22061,7 +22061,7 @@
         <v>151</v>
       </c>
       <c r="F108" s="157" t="n">
-        <v>4.02</v>
+        <v>6.49</v>
       </c>
       <c r="G108" s="158" t="s">
         <v>96</v>
@@ -22197,15 +22197,15 @@
       </c>
       <c r="D111" s="167" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F123,Equations!G123)</f>
-        <v>36.2447826086957</v>
+        <v>9.0923664921466</v>
       </c>
       <c r="E111" s="168" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F124,Equations!G124)</f>
-        <v>37.8278260869565</v>
+        <v>9.52261780104712</v>
       </c>
       <c r="F111" s="169" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F125,Equations!G125)</f>
-        <v>39.4108695652174</v>
+        <v>9.95286910994764</v>
       </c>
       <c r="G111" s="158" t="s">
         <v>40</v>
@@ -22251,15 +22251,15 @@
       </c>
       <c r="D112" s="170" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F126,Equations!G126)</f>
-        <v>33.8447826086957</v>
+        <v>8.3403664921466</v>
       </c>
       <c r="E112" s="143" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F127,Equations!G127)</f>
-        <v>34.8278260869565</v>
+        <v>8.58261780104712</v>
       </c>
       <c r="F112" s="171" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F128,Equations!G128)</f>
-        <v>35.8108695652174</v>
+        <v>8.82486910994764</v>
       </c>
       <c r="G112" s="158" t="s">
         <v>40</v>
@@ -22305,15 +22305,15 @@
       </c>
       <c r="D113" s="170" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F129,Equations!G129)</f>
-        <v>61.842736318408</v>
+        <v>53.9462403697997</v>
       </c>
       <c r="E113" s="143" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F130,Equations!G130)</f>
-        <v>63.6540298507463</v>
+        <v>55.5262557781202</v>
       </c>
       <c r="F113" s="171" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F131,Equations!G131)</f>
-        <v>65.4653233830846</v>
+        <v>57.1062711864407</v>
       </c>
       <c r="G113" s="158" t="s">
         <v>40</v>
@@ -22359,15 +22359,15 @@
       </c>
       <c r="D114" s="172" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F132,Equations!G132)</f>
-        <v>59.442736318408</v>
+        <v>50.5862403697997</v>
       </c>
       <c r="E114" s="173" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F133,Equations!G133)</f>
-        <v>61.5540298507463</v>
+        <v>52.5862557781202</v>
       </c>
       <c r="F114" s="174" t="n">
         <f aca="false">IF($F$96="Option A",Equations!F134,Equations!G134)</f>
-        <v>63.8653233830846</v>
+        <v>54.8662711864407</v>
       </c>
       <c r="G114" s="158" t="s">
         <v>40</v>
@@ -23220,7 +23220,7 @@
       </c>
       <c r="F132" s="201" t="n">
         <f aca="false">F105</f>
-        <v>150</v>
+        <v>47</v>
       </c>
       <c r="G132" s="190" t="s">
         <v>96</v>
@@ -23275,7 +23275,7 @@
       </c>
       <c r="F133" s="201" t="n">
         <f aca="false">F106</f>
-        <v>11.5</v>
+        <v>19.1</v>
       </c>
       <c r="G133" s="190" t="s">
         <v>96</v>
@@ -23330,7 +23330,7 @@
       </c>
       <c r="F134" s="201" t="n">
         <f aca="false">F107</f>
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="G134" s="190" t="s">
         <v>96</v>
@@ -23385,7 +23385,7 @@
       </c>
       <c r="F135" s="205" t="n">
         <f aca="false">IF(F96="Option A","N/A",F108)</f>
-        <v>4.02</v>
+        <v>6.49</v>
       </c>
       <c r="G135" s="190" t="s">
         <v>96</v>
@@ -23562,7 +23562,7 @@
       </c>
       <c r="K138" s="206" t="n">
         <f aca="false">E111</f>
-        <v>37.8278260869565</v>
+        <v>9.52261780104712</v>
       </c>
       <c r="L138" s="200" t="s">
         <v>40</v>
@@ -23616,7 +23616,7 @@
       </c>
       <c r="K139" s="206" t="n">
         <f aca="false">E112</f>
-        <v>34.8278260869565</v>
+        <v>8.58261780104712</v>
       </c>
       <c r="L139" s="200" t="s">
         <v>40</v>
@@ -23670,7 +23670,7 @@
       </c>
       <c r="K140" s="206" t="n">
         <f aca="false">E113</f>
-        <v>63.6540298507463</v>
+        <v>55.5262557781202</v>
       </c>
       <c r="L140" s="200" t="s">
         <v>40</v>
@@ -23724,7 +23724,7 @@
       </c>
       <c r="K141" s="206" t="n">
         <f aca="false">E114</f>
-        <v>61.5540298507463</v>
+        <v>52.5862557781202</v>
       </c>
       <c r="L141" s="200" t="s">
         <v>40</v>
@@ -29775,11 +29775,11 @@
       </c>
       <c r="F119" s="254" t="n">
         <f aca="false">('Design Calculator'!F97-'Design Calculator'!F98)*1000/20</f>
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="G119" s="254" t="n">
         <f aca="false">('Design Calculator'!F97-'Design Calculator'!F98)*1000/20</f>
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="H119" s="239"/>
     </row>
@@ -29790,11 +29790,11 @@
       </c>
       <c r="F120" s="254" t="n">
         <f aca="false">2.48*F119/('Design Calculator'!F98-2.48)-F121</f>
-        <v>5.32926483110985</v>
+        <v>16.0910725618786</v>
       </c>
       <c r="G120" s="254" t="n">
         <f aca="false">2.48*G119/('Design Calculator'!F98-2.48)</f>
-        <v>11.4391143911439</v>
+        <v>19.0184049079755</v>
       </c>
       <c r="H120" s="239"/>
     </row>
@@ -29805,11 +29805,11 @@
       </c>
       <c r="F121" s="254" t="n">
         <f aca="false">(F119*'Design Calculator'!F98*2.46)/('Design Calculator'!F99*('Design Calculator'!F98-2.48))</f>
-        <v>6.10984956003406</v>
+        <v>2.92733234609689</v>
       </c>
       <c r="G121" s="254" t="n">
         <f aca="false">('Design Calculator'!F99-'Design Calculator'!F100)*1000/21</f>
-        <v>95.2380952380952</v>
+        <v>142.857142857143</v>
       </c>
       <c r="H121" s="239"/>
     </row>
@@ -29821,7 +29821,7 @@
       <c r="F122" s="243"/>
       <c r="G122" s="254" t="n">
         <f aca="false">2.46*G121/('Design Calculator'!F99-2.46)</f>
-        <v>3.74617387728996</v>
+        <v>6.32748598178919</v>
       </c>
       <c r="H122" s="239"/>
     </row>
@@ -29834,11 +29834,11 @@
       </c>
       <c r="F123" s="254" t="n">
         <f aca="false">2.41+('Design Calculator'!F105*((2.41/('Design Calculator'!F106+'Design Calculator'!F107))+(16/1000)))</f>
-        <v>8.05215246636771</v>
+        <v>3.87394217473287</v>
       </c>
       <c r="G123" s="254" t="n">
         <f aca="false">2.41+('Design Calculator'!F$105*((2.41/'Design Calculator'!F$106)+(16/1000)))</f>
-        <v>36.2447826086957</v>
+        <v>9.0923664921466</v>
       </c>
       <c r="H123" s="239"/>
     </row>
@@ -29851,11 +29851,11 @@
       </c>
       <c r="F124" s="254" t="n">
         <f aca="false">2.48+('Design Calculator'!F105*((2.48/('Design Calculator'!F106+'Design Calculator'!F107))+(20/1000)))</f>
-        <v>8.81632286995516</v>
+        <v>4.15262099308611</v>
       </c>
       <c r="G124" s="254" t="n">
         <f aca="false">2.48+('Design Calculator'!F$105*((2.48/'Design Calculator'!F$106)+(20/1000)))</f>
-        <v>37.8278260869565</v>
+        <v>9.52261780104712</v>
       </c>
       <c r="H124" s="239"/>
     </row>
@@ -29868,11 +29868,11 @@
       </c>
       <c r="F125" s="254" t="n">
         <f aca="false">2.55+('Design Calculator'!F105*((2.55/('Design Calculator'!F106+'Design Calculator'!F107))+(24/1000)))</f>
-        <v>9.5804932735426</v>
+        <v>4.43129981143935</v>
       </c>
       <c r="G125" s="254" t="n">
         <f aca="false">2.55+('Design Calculator'!F$105*((2.55/'Design Calculator'!F$106)+(24/1000)))</f>
-        <v>39.4108695652174</v>
+        <v>9.95286910994764</v>
       </c>
       <c r="H125" s="239"/>
     </row>
@@ -29883,11 +29883,11 @@
       </c>
       <c r="F126" s="254" t="n">
         <f aca="false">2.41*('Design Calculator'!F105+'Design Calculator'!F106+'Design Calculator'!F107)/('Design Calculator'!F106+'Design Calculator'!F107)</f>
-        <v>5.65215246636771</v>
+        <v>3.12194217473287</v>
       </c>
       <c r="G126" s="254" t="n">
         <f aca="false">2.41*('Design Calculator'!F$105+'Design Calculator'!F$106)/'Design Calculator'!F$106</f>
-        <v>33.8447826086957</v>
+        <v>8.3403664921466</v>
       </c>
       <c r="H126" s="239"/>
     </row>
@@ -29898,11 +29898,11 @@
       </c>
       <c r="F127" s="254" t="n">
         <f aca="false">2.48*('Design Calculator'!F105+'Design Calculator'!F106+'Design Calculator'!F107)/('Design Calculator'!F106+'Design Calculator'!F107)</f>
-        <v>5.81632286995516</v>
+        <v>3.21262099308611</v>
       </c>
       <c r="G127" s="254" t="n">
         <f aca="false">2.48*('Design Calculator'!F$105+'Design Calculator'!F$106)/'Design Calculator'!F$106</f>
-        <v>34.8278260869565</v>
+        <v>8.58261780104712</v>
       </c>
       <c r="H127" s="239"/>
     </row>
@@ -29913,11 +29913,11 @@
       </c>
       <c r="F128" s="254" t="n">
         <f aca="false">2.55*('Design Calculator'!F105+'Design Calculator'!F106+'Design Calculator'!F107)/('Design Calculator'!F106+'Design Calculator'!F107)</f>
-        <v>5.9804932735426</v>
+        <v>3.30329981143935</v>
       </c>
       <c r="G128" s="254" t="n">
         <f aca="false">2.55*('Design Calculator'!F$105+'Design Calculator'!F$106)/'Design Calculator'!F$106</f>
-        <v>35.8108695652174</v>
+        <v>8.82486910994764</v>
       </c>
       <c r="H128" s="239"/>
     </row>
@@ -29930,11 +29930,11 @@
       </c>
       <c r="F129" s="254" t="n">
         <f aca="false">2.39*('Design Calculator'!F105+'Design Calculator'!F106+'Design Calculator'!F107)/'Design Calculator'!F107</f>
-        <v>6.24985</v>
+        <v>3.51842142857143</v>
       </c>
       <c r="G129" s="254" t="n">
         <f aca="false">2.39*('Design Calculator'!F$107+'Design Calculator'!F$108)/'Design Calculator'!F$108</f>
-        <v>61.842736318408</v>
+        <v>53.9462403697997</v>
       </c>
       <c r="H129" s="239"/>
     </row>
@@ -29947,11 +29947,11 @@
       </c>
       <c r="F130" s="254" t="n">
         <f aca="false">2.46*('Design Calculator'!F$105+'Design Calculator'!F$106+'Design Calculator'!F$107)/'Design Calculator'!F$107</f>
-        <v>6.4329</v>
+        <v>3.62147142857143</v>
       </c>
       <c r="G130" s="254" t="n">
         <f aca="false">2.46*('Design Calculator'!F$107+'Design Calculator'!F$108)/'Design Calculator'!F$108</f>
-        <v>63.6540298507463</v>
+        <v>55.5262557781202</v>
       </c>
       <c r="H130" s="239"/>
     </row>
@@ -29964,11 +29964,11 @@
       </c>
       <c r="F131" s="254" t="n">
         <f aca="false">2.53*('Design Calculator'!F$105+'Design Calculator'!F$106+'Design Calculator'!F$107)/'Design Calculator'!F$107</f>
-        <v>6.61595</v>
+        <v>3.72452142857143</v>
       </c>
       <c r="G131" s="254" t="n">
         <f aca="false">2.53*('Design Calculator'!F$107+'Design Calculator'!F$108)/'Design Calculator'!F$108</f>
-        <v>65.4653233830846</v>
+        <v>57.1062711864407</v>
       </c>
       <c r="H131" s="239"/>
     </row>
@@ -29979,11 +29979,11 @@
       </c>
       <c r="F132" s="254" t="n">
         <f aca="false">2.39+(('Design Calculator'!F$105+'Design Calculator'!F$106)*((2.39/'Design Calculator'!F$107)-(24/1000)))</f>
-        <v>2.37385</v>
+        <v>1.93202142857143</v>
       </c>
       <c r="G132" s="254" t="n">
         <f aca="false">2.39+('Design Calculator'!F$107*((2.39/'Design Calculator'!F$108)-(24/1000)))</f>
-        <v>59.442736318408</v>
+        <v>50.5862403697997</v>
       </c>
       <c r="H132" s="239"/>
     </row>
@@ -29994,11 +29994,11 @@
       </c>
       <c r="F133" s="254" t="n">
         <f aca="false">2.46+(('Design Calculator'!F$105+'Design Calculator'!F$106)*((2.46/'Design Calculator'!F$107)-(21/1000)))</f>
-        <v>3.0414</v>
+        <v>2.23337142857143</v>
       </c>
       <c r="G133" s="254" t="n">
         <f aca="false">2.46+('Design Calculator'!F$107*((2.46/'Design Calculator'!F$108)-(21/1000)))</f>
-        <v>61.5540298507463</v>
+        <v>52.5862557781202</v>
       </c>
       <c r="H133" s="239"/>
     </row>
@@ -30009,11 +30009,11 @@
       </c>
       <c r="F134" s="254" t="n">
         <f aca="false">2.53+(('Design Calculator'!F$105+'Design Calculator'!F$106)*((2.53/'Design Calculator'!F$107)-(16/1000)))</f>
-        <v>4.03195</v>
+        <v>2.66692142857143</v>
       </c>
       <c r="G134" s="254" t="n">
         <f aca="false">2.53+('Design Calculator'!F$107*((2.53/'Design Calculator'!F$108)-(16/1000)))</f>
-        <v>63.8653233830846</v>
+        <v>54.8662711864407</v>
       </c>
       <c r="H134" s="239"/>
     </row>

</xml_diff>